<commit_message>
Added data import, fixed design typos, and corrected Excel
</commit_message>
<xml_diff>
--- a/TP2 2020i - datos prueba.xlsx
+++ b/TP2 2020i - datos prueba.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\OneDrive - TEC\IC-4301 - 2020i BD1\Tareas programadas\TP2 2020i\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jos\Desktop\BasesPRY2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="17115" windowHeight="9285"/>
+    <workbookView xWindow="240" yWindow="72" windowWidth="17112" windowHeight="9288"/>
   </bookViews>
   <sheets>
     <sheet name="Teatros" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="172">
   <si>
     <t>nombre</t>
   </si>
@@ -196,9 +196,6 @@
   </si>
   <si>
     <t>luneta derecha</t>
-  </si>
-  <si>
-    <t>La Comedia</t>
   </si>
   <si>
     <t>A</t>
@@ -543,7 +540,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -809,7 +806,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -847,8 +844,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -876,6 +871,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1184,26 +1191,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M167"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" customWidth="1"/>
-    <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" customWidth="1"/>
-    <col min="6" max="12" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="23.88671875" customWidth="1"/>
+    <col min="4" max="4" width="27.5546875" customWidth="1"/>
+    <col min="5" max="5" width="18.88671875" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+    <col min="7" max="7" width="44.88671875" customWidth="1"/>
+    <col min="8" max="12" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="2:8" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="20" t="s">
         <v>0</v>
       </c>
@@ -1223,10 +1232,10 @@
         <v>5</v>
       </c>
       <c r="H2" s="22" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" s="15" t="s">
         <v>25</v>
       </c>
@@ -1237,7 +1246,7 @@
         <v>31</v>
       </c>
       <c r="E3" s="16">
-        <v>2555985</v>
+        <v>22555985</v>
       </c>
       <c r="F3" s="18" t="s">
         <v>34</v>
@@ -1249,7 +1258,7 @@
         <v>23841182</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="8" t="s">
         <v>26</v>
       </c>
@@ -1260,7 +1269,7 @@
         <v>32</v>
       </c>
       <c r="E4" s="2">
-        <v>8888155</v>
+        <v>28888155</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>35</v>
@@ -1272,7 +1281,7 @@
         <v>58825560</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="10" t="s">
         <v>27</v>
       </c>
@@ -1283,7 +1292,7 @@
         <v>33</v>
       </c>
       <c r="E5" s="11">
-        <v>6646701</v>
+        <v>26646701</v>
       </c>
       <c r="F5" s="13" t="s">
         <v>36</v>
@@ -1295,21 +1304,21 @@
         <v>44404475</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-    </row>
-    <row r="8" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+    </row>
+    <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:8" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="20" t="s">
         <v>9</v>
       </c>
@@ -1329,7 +1338,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B10" s="15" t="s">
         <v>25</v>
       </c>
@@ -1349,7 +1358,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="8" t="s">
         <v>25</v>
       </c>
@@ -1369,7 +1378,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="8" t="s">
         <v>26</v>
       </c>
@@ -1389,7 +1398,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="10" t="s">
         <v>27</v>
       </c>
@@ -1409,20 +1418,20 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="31"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="31"/>
-    </row>
-    <row r="16" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B14" s="29"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="29"/>
+    </row>
+    <row r="16" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
         <v>9</v>
       </c>
@@ -1436,172 +1445,172 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="41">
         <v>43625</v>
       </c>
-      <c r="E18" s="29">
+      <c r="E18" s="42">
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="41">
         <v>43626</v>
       </c>
-      <c r="E19" s="29">
+      <c r="E19" s="42">
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="41">
         <v>43628</v>
       </c>
-      <c r="E20" s="29">
+      <c r="E20" s="42">
         <v>0.625</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="41">
         <v>43662</v>
       </c>
-      <c r="E21" s="29">
+      <c r="E21" s="42">
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="41">
         <v>43633</v>
       </c>
-      <c r="E22" s="29">
+      <c r="E22" s="42">
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="41">
         <v>43634</v>
       </c>
-      <c r="E23" s="29">
+      <c r="E23" s="42">
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="41">
         <v>43641</v>
       </c>
-      <c r="E24" s="29">
+      <c r="E24" s="42">
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="41">
         <v>43642</v>
       </c>
-      <c r="E25" s="29">
+      <c r="E25" s="42">
         <v>0.625</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="41">
         <v>43642</v>
       </c>
-      <c r="E26" s="29">
+      <c r="E26" s="42">
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27" s="41">
         <v>43639</v>
       </c>
-      <c r="E27" s="29">
+      <c r="E27" s="42">
         <v>0.875</v>
       </c>
     </row>
-    <row r="28" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B28" s="10" t="s">
         <v>27</v>
       </c>
       <c r="C28" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D28" s="12">
+      <c r="D28" s="43">
         <v>43676</v>
       </c>
-      <c r="E28" s="30">
+      <c r="E28" s="44">
         <v>0.875</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="34"/>
-    </row>
-    <row r="31" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="32"/>
+    </row>
+    <row r="31" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B31" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B32" s="20" t="s">
         <v>9</v>
       </c>
@@ -1609,7 +1618,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B33" s="15" t="s">
         <v>25</v>
       </c>
@@ -1617,7 +1626,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B34" s="8" t="s">
         <v>25</v>
       </c>
@@ -1625,7 +1634,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B35" s="8" t="s">
         <v>25</v>
       </c>
@@ -1633,7 +1642,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B36" s="8" t="s">
         <v>25</v>
       </c>
@@ -1641,7 +1650,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B37" s="8" t="s">
         <v>25</v>
       </c>
@@ -1649,7 +1658,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B38" s="8" t="s">
         <v>26</v>
       </c>
@@ -1657,7 +1666,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B39" s="8" t="s">
         <v>26</v>
       </c>
@@ -1665,7 +1674,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B40" s="8" t="s">
         <v>26</v>
       </c>
@@ -1673,24 +1682,24 @@
         <v>58</v>
       </c>
     </row>
-    <row r="41" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B41" s="10" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
       <c r="C41" s="14" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B42" s="31"/>
-      <c r="C42" s="31"/>
-    </row>
-    <row r="44" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B42" s="29"/>
+      <c r="C42" s="29"/>
+    </row>
+    <row r="44" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B44" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="2:5" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:5" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B45" s="20" t="s">
         <v>9</v>
       </c>
@@ -1704,7 +1713,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B46" s="15" t="s">
         <v>25</v>
       </c>
@@ -1718,7 +1727,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B47" s="8" t="s">
         <v>25</v>
       </c>
@@ -1732,7 +1741,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B48" s="8" t="s">
         <v>25</v>
       </c>
@@ -1746,7 +1755,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B49" s="8" t="s">
         <v>25</v>
       </c>
@@ -1760,7 +1769,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B50" s="8" t="s">
         <v>25</v>
       </c>
@@ -1774,7 +1783,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B51" s="8" t="s">
         <v>25</v>
       </c>
@@ -1788,7 +1797,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B52" s="8" t="s">
         <v>25</v>
       </c>
@@ -1802,7 +1811,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B53" s="8" t="s">
         <v>25</v>
       </c>
@@ -1816,7 +1825,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B54" s="8" t="s">
         <v>25</v>
       </c>
@@ -1830,7 +1839,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B55" s="8" t="s">
         <v>25</v>
       </c>
@@ -1844,7 +1853,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B56" s="8" t="s">
         <v>26</v>
       </c>
@@ -1858,7 +1867,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B57" s="8" t="s">
         <v>26</v>
       </c>
@@ -1872,7 +1881,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B58" s="8" t="s">
         <v>26</v>
       </c>
@@ -1886,7 +1895,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="59" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B59" s="10" t="s">
         <v>27</v>
       </c>
@@ -1900,18 +1909,18 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B60" s="31"/>
-      <c r="C60" s="31"/>
-      <c r="D60" s="31"/>
-      <c r="E60" s="31"/>
-    </row>
-    <row r="62" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B60" s="29"/>
+      <c r="C60" s="29"/>
+      <c r="D60" s="29"/>
+      <c r="E60" s="29"/>
+    </row>
+    <row r="62" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B62" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="63" spans="2:5" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:5" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B63" s="20" t="s">
         <v>9</v>
       </c>
@@ -1925,7 +1934,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B64" s="15" t="s">
         <v>25</v>
       </c>
@@ -1933,13 +1942,13 @@
         <v>51</v>
       </c>
       <c r="D64" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E64" s="19">
         <v>24</v>
       </c>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B65" s="8" t="s">
         <v>25</v>
       </c>
@@ -1947,13 +1956,13 @@
         <v>51</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E65" s="9">
         <v>24</v>
       </c>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B66" s="8" t="s">
         <v>25</v>
       </c>
@@ -1961,13 +1970,13 @@
         <v>51</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E66" s="9">
         <v>24</v>
       </c>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B67" s="8" t="s">
         <v>25</v>
       </c>
@@ -1975,13 +1984,13 @@
         <v>51</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E67" s="9">
         <v>24</v>
       </c>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B68" s="8" t="s">
         <v>25</v>
       </c>
@@ -1989,13 +1998,13 @@
         <v>51</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E68" s="9">
         <v>26</v>
       </c>
     </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B69" s="8" t="s">
         <v>25</v>
       </c>
@@ -2003,13 +2012,13 @@
         <v>51</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E69" s="9">
         <v>26</v>
       </c>
     </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B70" s="8" t="s">
         <v>25</v>
       </c>
@@ -2017,13 +2026,13 @@
         <v>51</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E70" s="9">
         <v>26</v>
       </c>
     </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B71" s="8" t="s">
         <v>25</v>
       </c>
@@ -2031,13 +2040,13 @@
         <v>51</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E71" s="9">
         <v>26</v>
       </c>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B72" s="8" t="s">
         <v>25</v>
       </c>
@@ -2045,13 +2054,13 @@
         <v>51</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E72" s="9">
         <v>24</v>
       </c>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B73" s="8" t="s">
         <v>25</v>
       </c>
@@ -2059,13 +2068,13 @@
         <v>51</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E73" s="9">
         <v>24</v>
       </c>
     </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B74" s="8" t="s">
         <v>25</v>
       </c>
@@ -2073,13 +2082,13 @@
         <v>51</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E74" s="9">
         <v>22</v>
       </c>
     </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B75" s="8" t="s">
         <v>25</v>
       </c>
@@ -2087,13 +2096,13 @@
         <v>51</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E75" s="9">
         <v>20</v>
       </c>
     </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B76" s="8" t="s">
         <v>25</v>
       </c>
@@ -2101,13 +2110,13 @@
         <v>51</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E76" s="9">
         <v>18</v>
       </c>
     </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B77" s="8" t="s">
         <v>25</v>
       </c>
@@ -2115,13 +2124,13 @@
         <v>51</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E77" s="9">
         <v>14</v>
       </c>
     </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B78" s="8" t="s">
         <v>25</v>
       </c>
@@ -2129,13 +2138,13 @@
         <v>52</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E78" s="9">
         <v>30</v>
       </c>
     </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B79" s="8" t="s">
         <v>25</v>
       </c>
@@ -2143,13 +2152,13 @@
         <v>52</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E79" s="9">
         <v>30</v>
       </c>
     </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B80" s="8" t="s">
         <v>25</v>
       </c>
@@ -2157,13 +2166,13 @@
         <v>52</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E80" s="9">
         <v>32</v>
       </c>
     </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B81" s="8" t="s">
         <v>25</v>
       </c>
@@ -2171,13 +2180,13 @@
         <v>52</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E81" s="9">
         <v>42</v>
       </c>
     </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B82" s="8" t="s">
         <v>25</v>
       </c>
@@ -2185,13 +2194,13 @@
         <v>53</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E82" s="9">
         <v>12</v>
       </c>
     </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B83" s="8" t="s">
         <v>25</v>
       </c>
@@ -2199,13 +2208,13 @@
         <v>53</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E83" s="9">
         <v>14</v>
       </c>
     </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B84" s="8" t="s">
         <v>25</v>
       </c>
@@ -2213,13 +2222,13 @@
         <v>53</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E84" s="9">
         <v>13</v>
       </c>
     </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B85" s="8" t="s">
         <v>25</v>
       </c>
@@ -2227,13 +2236,13 @@
         <v>53</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E85" s="9">
         <v>12</v>
       </c>
     </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B86" s="8" t="s">
         <v>25</v>
       </c>
@@ -2241,13 +2250,13 @@
         <v>53</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E86" s="9">
         <v>12</v>
       </c>
     </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B87" s="8" t="s">
         <v>25</v>
       </c>
@@ -2255,13 +2264,13 @@
         <v>54</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E87" s="9">
         <v>21</v>
       </c>
     </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B88" s="8" t="s">
         <v>25</v>
       </c>
@@ -2269,13 +2278,13 @@
         <v>54</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E88" s="9">
         <v>24</v>
       </c>
     </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B89" s="8" t="s">
         <v>25</v>
       </c>
@@ -2283,13 +2292,13 @@
         <v>54</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E89" s="9">
         <v>27</v>
       </c>
     </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B90" s="8" t="s">
         <v>25</v>
       </c>
@@ -2297,13 +2306,13 @@
         <v>54</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E90" s="9">
         <v>30</v>
       </c>
     </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B91" s="8" t="s">
         <v>25</v>
       </c>
@@ -2311,13 +2320,13 @@
         <v>54</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E91" s="9">
         <v>30</v>
       </c>
     </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B92" s="8" t="s">
         <v>25</v>
       </c>
@@ -2325,13 +2334,13 @@
         <v>55</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E92" s="9">
         <v>12</v>
       </c>
     </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B93" s="8" t="s">
         <v>25</v>
       </c>
@@ -2339,13 +2348,13 @@
         <v>55</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E93" s="9">
         <v>14</v>
       </c>
     </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B94" s="8" t="s">
         <v>25</v>
       </c>
@@ -2353,13 +2362,13 @@
         <v>55</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E94" s="9">
         <v>13</v>
       </c>
     </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B95" s="8" t="s">
         <v>25</v>
       </c>
@@ -2367,13 +2376,13 @@
         <v>55</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E95" s="9">
         <v>12</v>
       </c>
     </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B96" s="8" t="s">
         <v>25</v>
       </c>
@@ -2381,13 +2390,13 @@
         <v>55</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E96" s="9">
         <v>12</v>
       </c>
     </row>
-    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B97" s="8" t="s">
         <v>26</v>
       </c>
@@ -2395,13 +2404,13 @@
         <v>56</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E97" s="9">
         <v>11</v>
       </c>
     </row>
-    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B98" s="8" t="s">
         <v>26</v>
       </c>
@@ -2409,13 +2418,13 @@
         <v>56</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E98" s="9">
         <v>10</v>
       </c>
     </row>
-    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B99" s="8" t="s">
         <v>26</v>
       </c>
@@ -2423,13 +2432,13 @@
         <v>56</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E99" s="9">
         <v>11</v>
       </c>
     </row>
-    <row r="100" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B100" s="8" t="s">
         <v>26</v>
       </c>
@@ -2437,13 +2446,13 @@
         <v>56</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E100" s="9">
         <v>10</v>
       </c>
     </row>
-    <row r="101" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B101" s="8" t="s">
         <v>26</v>
       </c>
@@ -2451,13 +2460,13 @@
         <v>56</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E101" s="9">
         <v>11</v>
       </c>
     </row>
-    <row r="102" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B102" s="8" t="s">
         <v>26</v>
       </c>
@@ -2465,13 +2474,13 @@
         <v>56</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E102" s="9">
         <v>10</v>
       </c>
     </row>
-    <row r="103" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B103" s="8" t="s">
         <v>26</v>
       </c>
@@ -2479,13 +2488,13 @@
         <v>56</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E103" s="9">
         <v>11</v>
       </c>
     </row>
-    <row r="104" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B104" s="8" t="s">
         <v>26</v>
       </c>
@@ -2493,13 +2502,13 @@
         <v>56</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E104" s="9">
         <v>10</v>
       </c>
     </row>
-    <row r="105" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B105" s="8" t="s">
         <v>26</v>
       </c>
@@ -2507,13 +2516,13 @@
         <v>56</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E105" s="9">
         <v>11</v>
       </c>
     </row>
-    <row r="106" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B106" s="8" t="s">
         <v>26</v>
       </c>
@@ -2521,13 +2530,13 @@
         <v>57</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E106" s="9">
         <v>12</v>
       </c>
     </row>
-    <row r="107" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B107" s="8" t="s">
         <v>26</v>
       </c>
@@ -2535,13 +2544,13 @@
         <v>57</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E107" s="9">
         <v>11</v>
       </c>
     </row>
-    <row r="108" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B108" s="8" t="s">
         <v>26</v>
       </c>
@@ -2549,13 +2558,13 @@
         <v>57</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E108" s="9">
         <v>12</v>
       </c>
     </row>
-    <row r="109" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B109" s="8" t="s">
         <v>26</v>
       </c>
@@ -2563,13 +2572,13 @@
         <v>57</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E109" s="9">
         <v>11</v>
       </c>
     </row>
-    <row r="110" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B110" s="8" t="s">
         <v>26</v>
       </c>
@@ -2577,13 +2586,13 @@
         <v>57</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E110" s="9">
         <v>12</v>
       </c>
     </row>
-    <row r="111" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B111" s="8" t="s">
         <v>26</v>
       </c>
@@ -2591,13 +2600,13 @@
         <v>57</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E111" s="9">
         <v>11</v>
       </c>
     </row>
-    <row r="112" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B112" s="8" t="s">
         <v>26</v>
       </c>
@@ -2605,13 +2614,13 @@
         <v>57</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E112" s="9">
         <v>12</v>
       </c>
     </row>
-    <row r="113" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B113" s="8" t="s">
         <v>26</v>
       </c>
@@ -2619,13 +2628,13 @@
         <v>57</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E113" s="9">
         <v>11</v>
       </c>
     </row>
-    <row r="114" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B114" s="8" t="s">
         <v>26</v>
       </c>
@@ -2633,13 +2642,13 @@
         <v>57</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E114" s="9">
         <v>12</v>
       </c>
     </row>
-    <row r="115" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B115" s="8" t="s">
         <v>26</v>
       </c>
@@ -2647,13 +2656,13 @@
         <v>57</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E115" s="9">
         <v>11</v>
       </c>
     </row>
-    <row r="116" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B116" s="8" t="s">
         <v>26</v>
       </c>
@@ -2661,13 +2670,13 @@
         <v>58</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E116" s="9">
         <v>11</v>
       </c>
     </row>
-    <row r="117" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B117" s="8" t="s">
         <v>26</v>
       </c>
@@ -2675,13 +2684,13 @@
         <v>58</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E117" s="9">
         <v>12</v>
       </c>
     </row>
-    <row r="118" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B118" s="8" t="s">
         <v>26</v>
       </c>
@@ -2689,13 +2698,13 @@
         <v>58</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E118" s="9">
         <v>13</v>
       </c>
     </row>
-    <row r="119" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B119" s="8" t="s">
         <v>26</v>
       </c>
@@ -2703,13 +2712,13 @@
         <v>58</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E119" s="9">
         <v>12</v>
       </c>
     </row>
-    <row r="120" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B120" s="8" t="s">
         <v>26</v>
       </c>
@@ -2717,13 +2726,13 @@
         <v>58</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E120" s="9">
         <v>11</v>
       </c>
     </row>
-    <row r="121" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B121" s="8" t="s">
         <v>26</v>
       </c>
@@ -2731,13 +2740,13 @@
         <v>58</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E121" s="9">
         <v>10</v>
       </c>
     </row>
-    <row r="122" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B122" s="8" t="s">
         <v>26</v>
       </c>
@@ -2745,13 +2754,13 @@
         <v>58</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E122" s="9">
         <v>11</v>
       </c>
     </row>
-    <row r="123" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B123" s="8" t="s">
         <v>26</v>
       </c>
@@ -2759,13 +2768,13 @@
         <v>58</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E123" s="9">
         <v>13</v>
       </c>
     </row>
-    <row r="124" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B124" s="8" t="s">
         <v>26</v>
       </c>
@@ -2773,13 +2782,13 @@
         <v>58</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E124" s="9">
         <v>12</v>
       </c>
     </row>
-    <row r="125" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B125" s="8" t="s">
         <v>26</v>
       </c>
@@ -2787,13 +2796,13 @@
         <v>58</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E125" s="9">
         <v>12</v>
       </c>
     </row>
-    <row r="126" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B126" s="8" t="s">
         <v>27</v>
       </c>
@@ -2801,13 +2810,13 @@
         <v>52</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E126" s="9">
         <v>18</v>
       </c>
     </row>
-    <row r="127" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B127" s="8" t="s">
         <v>27</v>
       </c>
@@ -2815,13 +2824,13 @@
         <v>52</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E127" s="9">
         <v>20</v>
       </c>
     </row>
-    <row r="128" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B128" s="8" t="s">
         <v>27</v>
       </c>
@@ -2829,13 +2838,13 @@
         <v>52</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E128" s="9">
         <v>22</v>
       </c>
     </row>
-    <row r="129" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B129" s="8" t="s">
         <v>27</v>
       </c>
@@ -2843,13 +2852,13 @@
         <v>52</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E129" s="9">
         <v>14</v>
       </c>
     </row>
-    <row r="130" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B130" s="10" t="s">
         <v>27</v>
       </c>
@@ -2857,55 +2866,55 @@
         <v>52</v>
       </c>
       <c r="D130" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E130" s="14">
         <v>14</v>
       </c>
     </row>
-    <row r="133" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B133" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="134" spans="2:13" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="134" spans="2:13" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B134" s="20" t="s">
         <v>0</v>
       </c>
       <c r="C134" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="D134" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="D134" s="21" t="s">
+      <c r="E134" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="E134" s="21" t="s">
+      <c r="F134" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="F134" s="21" t="s">
+      <c r="G134" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="H134" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="G134" s="21" t="s">
+      <c r="I134" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="J134" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="H134" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="I134" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="J134" s="21" t="s">
+      <c r="K134" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="K134" s="21" t="s">
+      <c r="L134" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="L134" s="22" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="135" spans="2:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="135" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B135" s="15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C135" s="16">
         <v>109450564</v>
@@ -2914,10 +2923,10 @@
         <v>29259</v>
       </c>
       <c r="E135" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F135" s="16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G135" s="16">
         <v>86320431</v>
@@ -2929,18 +2938,18 @@
         <v>65119247</v>
       </c>
       <c r="J135" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="K135" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="K135" s="16" t="s">
+      <c r="L135" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="L135" s="19" t="s">
+    </row>
+    <row r="136" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B136" s="10" t="s">
         <v>157</v>
-      </c>
-    </row>
-    <row r="136" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B136" s="10" t="s">
-        <v>158</v>
       </c>
       <c r="C136" s="11">
         <v>206710046</v>
@@ -2949,10 +2958,10 @@
         <v>31076</v>
       </c>
       <c r="E136" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F136" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G136" s="11">
         <v>98712584</v>
@@ -2964,21 +2973,21 @@
         <v>88760431</v>
       </c>
       <c r="J136" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K136" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L136" s="14" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="139" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="139" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B139" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="140" spans="2:13" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="140" spans="2:13" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B140" s="20" t="s">
         <v>9</v>
       </c>
@@ -2986,37 +2995,37 @@
         <v>0</v>
       </c>
       <c r="D140" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="E140" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="E140" s="21" t="s">
+      <c r="F140" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="F140" s="21" t="s">
+      <c r="G140" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="G140" s="21" t="s">
+      <c r="H140" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="I140" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="H140" s="21" t="s">
+      <c r="J140" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="K140" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="I140" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="J140" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="K140" s="21" t="s">
+      <c r="L140" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="L140" s="21" t="s">
+      <c r="M140" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="M140" s="22" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="141" spans="2:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="141" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B141" s="15" t="s">
         <v>25</v>
       </c>
@@ -3030,10 +3039,10 @@
         <v>17664</v>
       </c>
       <c r="F141" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G141" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H141" s="16">
         <v>91178174</v>
@@ -3041,21 +3050,21 @@
       <c r="I141" s="16"/>
       <c r="J141" s="16"/>
       <c r="K141" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L141" s="16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M141" s="19" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="142" spans="2:13" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="142" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B142" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D142" s="2">
         <v>113290303</v>
@@ -3064,10 +3073,10 @@
         <v>22559</v>
       </c>
       <c r="F142" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G142" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H142" s="2">
         <v>84260976</v>
@@ -3079,16 +3088,16 @@
         <v>71915451</v>
       </c>
       <c r="K142" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L142" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M142" s="9" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="143" spans="2:13" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="143" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B143" s="8" t="s">
         <v>26</v>
       </c>
@@ -3102,10 +3111,10 @@
         <v>20132</v>
       </c>
       <c r="F143" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G143" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H143" s="2">
         <v>42095437</v>
@@ -3113,21 +3122,21 @@
       <c r="I143" s="2"/>
       <c r="J143" s="2"/>
       <c r="K143" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L143" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M143" s="9" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="144" spans="2:13" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="144" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B144" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D144" s="2">
         <v>305290334</v>
@@ -3136,10 +3145,10 @@
         <v>30146</v>
       </c>
       <c r="F144" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G144" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H144" s="2">
         <v>83556451</v>
@@ -3149,16 +3158,16 @@
       </c>
       <c r="J144" s="2"/>
       <c r="K144" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L144" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M144" s="9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="145" spans="2:13" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="145" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B145" s="8" t="s">
         <v>27</v>
       </c>
@@ -3172,10 +3181,10 @@
         <v>17526</v>
       </c>
       <c r="F145" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G145" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H145" s="2">
         <v>64409720</v>
@@ -3183,21 +3192,21 @@
       <c r="I145" s="2"/>
       <c r="J145" s="2"/>
       <c r="K145" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L145" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M145" s="9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="146" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="146" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B146" s="10" t="s">
         <v>27</v>
       </c>
       <c r="C146" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D146" s="11">
         <v>402950337</v>
@@ -3206,10 +3215,10 @@
         <v>30724</v>
       </c>
       <c r="F146" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G146" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H146" s="11">
         <v>83945052</v>
@@ -3217,21 +3226,21 @@
       <c r="I146" s="11"/>
       <c r="J146" s="11"/>
       <c r="K146" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L146" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="M146" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="M146" s="14" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="149" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="149" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B149" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="150" spans="2:13" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="150" spans="2:13" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B150" s="20" t="s">
         <v>9</v>
       </c>
@@ -3239,42 +3248,42 @@
         <v>0</v>
       </c>
       <c r="D150" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="E150" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="E150" s="21" t="s">
+      <c r="F150" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="F150" s="21" t="s">
+      <c r="G150" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="G150" s="21" t="s">
+      <c r="H150" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="I150" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="H150" s="21" t="s">
+      <c r="J150" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="K150" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="I150" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="J150" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="K150" s="21" t="s">
+      <c r="L150" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="L150" s="21" t="s">
+      <c r="M150" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="M150" s="22" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="151" spans="2:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="151" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B151" s="15" t="s">
         <v>25</v>
       </c>
       <c r="C151" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D151" s="16">
         <v>111500626</v>
@@ -3283,10 +3292,10 @@
         <v>27761</v>
       </c>
       <c r="F151" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G151" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H151" s="16">
         <v>85302637</v>
@@ -3294,21 +3303,21 @@
       <c r="I151" s="16"/>
       <c r="J151" s="16"/>
       <c r="K151" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="L151" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="M151" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="L151" s="16" t="s">
+    </row>
+    <row r="152" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B152" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C152" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="M151" s="19" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="152" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B152" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C152" s="2" t="s">
-        <v>121</v>
       </c>
       <c r="D152" s="2">
         <v>302420072</v>
@@ -3317,10 +3326,10 @@
         <v>27370</v>
       </c>
       <c r="F152" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G152" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H152" s="2">
         <v>64066575</v>
@@ -3330,21 +3339,21 @@
       </c>
       <c r="J152" s="2"/>
       <c r="K152" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L152" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M152" s="9" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="153" spans="2:13" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="153" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B153" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D153" s="2">
         <v>207150434</v>
@@ -3353,10 +3362,10 @@
         <v>18194</v>
       </c>
       <c r="F153" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G153" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H153" s="2">
         <v>84049313</v>
@@ -3364,21 +3373,21 @@
       <c r="I153" s="2"/>
       <c r="J153" s="2"/>
       <c r="K153" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L153" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M153" s="9" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="154" spans="2:13" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="154" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B154" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D154" s="2">
         <v>103107916</v>
@@ -3387,10 +3396,10 @@
         <v>26356</v>
       </c>
       <c r="F154" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G154" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H154" s="2">
         <v>55806498</v>
@@ -3400,21 +3409,21 @@
         <v>82997979</v>
       </c>
       <c r="K154" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L154" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M154" s="9" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="155" spans="2:13" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="155" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B155" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D155" s="2">
         <v>306290526</v>
@@ -3423,10 +3432,10 @@
         <v>34787</v>
       </c>
       <c r="F155" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G155" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H155" s="2">
         <v>84062795</v>
@@ -3438,21 +3447,21 @@
         <v>98341131</v>
       </c>
       <c r="K155" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L155" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M155" s="9" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="156" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="156" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B156" s="10" t="s">
         <v>27</v>
       </c>
       <c r="C156" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D156" s="11">
         <v>111490429</v>
@@ -3461,10 +3470,10 @@
         <v>32669</v>
       </c>
       <c r="F156" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G156" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H156" s="11">
         <v>64196092</v>
@@ -3472,21 +3481,21 @@
       <c r="I156" s="11"/>
       <c r="J156" s="11"/>
       <c r="K156" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L156" s="11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M156" s="14" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="159" spans="2:13" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="159" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B159" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="160" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="160" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B160" s="1" t="s">
         <v>0</v>
       </c>
@@ -3494,104 +3503,104 @@
         <v>3</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E160" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F160" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="F160" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="161" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="161" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B161" s="26" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C161" s="27">
         <v>89571024</v>
       </c>
       <c r="D161" s="28" t="s">
-        <v>148</v>
-      </c>
-      <c r="E161" s="35" t="s">
-        <v>164</v>
-      </c>
-      <c r="F161" s="36">
+        <v>147</v>
+      </c>
+      <c r="E161" s="33" t="s">
+        <v>163</v>
+      </c>
+      <c r="F161" s="34">
         <v>286</v>
       </c>
     </row>
-    <row r="162" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B162" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C162" s="16">
         <v>76955860</v>
       </c>
       <c r="D162" s="25" t="s">
-        <v>149</v>
-      </c>
-      <c r="E162" s="37" t="s">
-        <v>165</v>
-      </c>
-      <c r="F162" s="38">
+        <v>148</v>
+      </c>
+      <c r="E162" s="35" t="s">
+        <v>164</v>
+      </c>
+      <c r="F162" s="36">
         <v>831</v>
       </c>
     </row>
-    <row r="163" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B163" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C163" s="2">
         <v>94890535</v>
       </c>
       <c r="D163" s="23" t="s">
-        <v>150</v>
-      </c>
-      <c r="E163" s="39" t="s">
-        <v>166</v>
-      </c>
-      <c r="F163" s="40">
+        <v>149</v>
+      </c>
+      <c r="E163" s="37" t="s">
+        <v>165</v>
+      </c>
+      <c r="F163" s="38">
         <v>492</v>
       </c>
     </row>
-    <row r="164" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B164" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C164" s="2">
         <v>84417390</v>
       </c>
       <c r="D164" s="23" t="s">
-        <v>151</v>
-      </c>
-      <c r="E164" s="39" t="s">
-        <v>163</v>
-      </c>
-      <c r="F164" s="40">
+        <v>150</v>
+      </c>
+      <c r="E164" s="37" t="s">
+        <v>162</v>
+      </c>
+      <c r="F164" s="38">
         <v>231</v>
       </c>
     </row>
-    <row r="165" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B165" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C165" s="11">
         <v>61787392</v>
       </c>
       <c r="D165" s="24" t="s">
-        <v>152</v>
-      </c>
-      <c r="E165" s="41" t="s">
-        <v>167</v>
-      </c>
-      <c r="F165" s="42">
+        <v>151</v>
+      </c>
+      <c r="E165" s="39" t="s">
+        <v>166</v>
+      </c>
+      <c r="F165" s="40">
         <v>817</v>
       </c>
     </row>
-    <row r="166" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B166" s="1"/>
     </row>
-    <row r="167" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B167" s="1"/>
     </row>
   </sheetData>

</xml_diff>